<commit_message>
the program will now read the pdf, assign the data to variables, and create a new excel file containing the data
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -356,9 +356,77 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t xml:space="preserve">240404929
+</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Pro 8200S</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>- 96cpm (B&amp;W) Includes: 200-sheet ADF, duplex unit, 3,000 sheets of paper capacity, and 2 x 250GB HDD. Toner &amp; Developer not included with mainframe and must be added to initial order. Max Monthly Vol 1M. Requires Surge Protector (241007138MIU) &amp; Pro Toner 8200S(244828484), as well as one of the following Finoshers SR5050 (241404548) or SR5060 (241404550) or SK5030 Stacker (241404656).</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>26,488</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>23,839</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>22,514</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>48,011</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
           <t xml:space="preserve">
 240404930
 </t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Pro 8210S</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>- 111cpm (B&amp;W) Includes: 200-sheet ADF, duplex unit, 3,000 sheets of paper capacity, and 2 x 250GB HDD. Toner &amp; Developer not included with mainframe and must be added to initial order. Max Monthly Vol 1M. Requires Surge Protector (241007138MIU) &amp; Pro Toner 8200S(244828484), as well as one of the following Finoshers SR5050 (241404548) or SR5060 (241404550) or SK5030 Stacker (241404656).</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>33,285</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>29,957</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>28,293</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">s59,880 </t>
         </is>
       </c>
     </row>

</xml_diff>